<commit_message>
Nueva red de alcantarillado para diseñar
Se modificaron los datos adaptándolos a la nueva red de prueba
</commit_message>
<xml_diff>
--- a/Diseño de alcantarillado/aux_entradas.xlsx
+++ b/Diseño de alcantarillado/aux_entradas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitHub\Aplicacion-Hidraulica\Diseño de alcantarillado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitHub\Aplicacion-Civil-Hidraulica\Diseño de alcantarillado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7B5531-300A-4AE8-ADAE-4330EDC08BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5906A9-A8C3-4B9B-943B-47374C6343A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,31 +57,8 @@
 (mm)</t>
   </si>
   <si>
-    <r>
-      <t>Caudal individual
-(m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/s)</t>
-    </r>
+    <t>Caudal individual
+(L/s)</t>
   </si>
 </sst>
 </file>
@@ -89,18 +66,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,17 +113,14 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+      <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
@@ -171,6 +137,9 @@
           <xfpb:DXFComplement i="0"/>
         </ext>
       </extLst>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -208,24 +177,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{919CC8D5-69E7-47A8-BF0A-C0554C8AC87C}" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{919CC8D5-69E7-47A8-BF0A-C0554C8AC87C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{919CC8D5-69E7-47A8-BF0A-C0554C8AC87C}" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{919CC8D5-69E7-47A8-BF0A-C0554C8AC87C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{494DECD4-9A46-472A-9B3C-372F399F2213}" name="No."/>
-    <tableColumn id="2" xr3:uid="{23187485-5E1A-4E7E-AAA5-4364F2FBBF2F}" name="Cota_x000a_(m. s. n. m.)" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{379C0DB9-5134-454B-BA94-F7A046D40C9F}" name="Cabecera" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{23187485-5E1A-4E7E-AAA5-4364F2FBBF2F}" name="Cota_x000a_(m. s. n. m.)" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{379C0DB9-5134-454B-BA94-F7A046D40C9F}" name="Cabecera" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0103BC3F-BA3B-4CF3-92B5-39FCC76AC6BB}" name="Table3" displayName="Table3" ref="A1:F3" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:F3" xr:uid="{0103BC3F-BA3B-4CF3-92B5-39FCC76AC6BB}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0103BC3F-BA3B-4CF3-92B5-39FCC76AC6BB}" name="Table3" displayName="Table3" ref="A1:F7" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F7" xr:uid="{0103BC3F-BA3B-4CF3-92B5-39FCC76AC6BB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -237,9 +206,9 @@
     <tableColumn id="1" xr3:uid="{19964BAB-6AE5-420F-A963-AB7177EFB311}" name="No."/>
     <tableColumn id="2" xr3:uid="{428F2B22-08BC-41D9-8E88-31672DCB82E9}" name="Pozo inicial"/>
     <tableColumn id="3" xr3:uid="{90242C70-8700-4FDF-9256-69FCDBD2B78B}" name="Pozo final"/>
-    <tableColumn id="6" xr3:uid="{1149F6ED-FA12-4AE4-BA24-07055E2FC6CD}" name="Caudal individual_x000a_(m3/s)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{E8A322F8-6450-4DD3-9D1B-AA0FBD180EAF}" name="Longitud horizontal_x000a_(m)" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{88CADDF7-906F-4188-8F97-DEDE719947B3}" name="Rugosidad absoluta_x000a_(mm)" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1149F6ED-FA12-4AE4-BA24-07055E2FC6CD}" name="Caudal individual_x000a_(L/s)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{E8A322F8-6450-4DD3-9D1B-AA0FBD180EAF}" name="Longitud horizontal_x000a_(m)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{88CADDF7-906F-4188-8F97-DEDE719947B3}" name="Rugosidad absoluta_x000a_(mm)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -525,10 +494,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,10 +522,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>2995.5</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,10 +533,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>2997</v>
+        <v>1001</v>
       </c>
       <c r="C3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -575,10 +544,54 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>3000</v>
+        <v>998</v>
       </c>
       <c r="C4" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>997</v>
+      </c>
+      <c r="C5" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>997.5</v>
+      </c>
+      <c r="C6" s="4" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>996</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>994</v>
+      </c>
+      <c r="C8" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -595,10 +608,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +623,7 @@
     <col min="6" max="6" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,16 +648,16 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
       <c r="D2" s="3">
-        <v>1.75</v>
+        <v>50</v>
       </c>
       <c r="E2" s="3">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F2" s="5">
         <v>1.5E-3</v>
@@ -658,15 +671,95 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3">
-        <v>1.5</v>
+        <v>100</v>
       </c>
       <c r="E3" s="3">
+        <v>80</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>150</v>
+      </c>
+      <c r="E4" s="3">
         <v>50</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F4" s="5">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>100</v>
+      </c>
+      <c r="E5" s="3">
+        <v>60</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>150</v>
+      </c>
+      <c r="E6" s="3">
+        <v>50</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3">
+        <v>50</v>
+      </c>
+      <c r="E7" s="3">
+        <v>80</v>
+      </c>
+      <c r="F7" s="5">
         <v>1.5E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nueva red de prueba
Se modificaron los datos para probar el diseño en otra red de alcantarillado
</commit_message>
<xml_diff>
--- a/Diseño de alcantarillado/aux_entradas.xlsx
+++ b/Diseño de alcantarillado/aux_entradas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitHub\Aplicacion-Civil-Hidraulica\Diseño de alcantarillado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5906A9-A8C3-4B9B-943B-47374C6343A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5492C8BA-A2A5-4D4C-A121-AE2925E23273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMACIÓN_POZOS" sheetId="2" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,8 +778,8 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>